<commit_message>
Added groups and java docs to the test
</commit_message>
<xml_diff>
--- a/src/main/java/reports/TestFailure.xlsx
+++ b/src/main/java/reports/TestFailure.xlsx
@@ -23,17 +23,10 @@
     <t>Log Message</t>
   </si>
   <si>
-    <t>addOrSubtractItem</t>
+    <t>searchCategory</t>
   </si>
   <si>
-    <t>org.openqa.selenium.NoSuchElementException: An element could not be located on the page using the given search parameters.
-For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Build info: version: '4.20.0', revision: '866c76ca80'
-System info: os.name: 'Mac OS X', os.arch: 'aarch64', os.version: '14.3', java.version: '11.0.23'
-Driver info: io.appium.java_client.android.AndroidDriver
-Command: [ede3bb74-6ca4-4fd7-8030-7065044e798d, findElement {using=xpath, value=//android.widget.TextView[@resource-id='com.zopsmart.stg.scarlet:id/tv_quantity']}]
-Capabilities {appium:app: /Users/raramuri/zs-appium-a..., appium:appActivity: com.zopsmart.platformapplic..., appium:appPackage: com.zopsmart.stg.scarlet, appium:automationName: UIAutomator2, appium:databaseEnabled: false, appium:desired: {app: /Users/raramuri/zs-appium-a..., appActivity: com.zopsmart.platformapplic..., automationName: UIAutomator2, deviceName: emulator-5554, platformName: ANDROID}, appium:deviceApiLevel: 30, appium:deviceManufacturer: Google, appium:deviceModel: sdk_gphone_arm64, appium:deviceName: emulator-5554, appium:deviceScreenDensity: 440, appium:deviceScreenSize: 1080x2220, appium:deviceUDID: emulator-5554, appium:javascriptEnabled: true, appium:locationContextEnabled: false, appium:networkConnectionEnabled: true, appium:pixelRatio: 2.75, appium:platformVersion: 11, appium:statBarHeight: 66, appium:takesScreenshot: true, appium:viewportRect: {height: 2154, left: 0, top: 66, width: 1080}, appium:warnings: {}, appium:webStorageEnabled: false, platformName: ANDROID}
-Session ID: ede3bb74-6ca4-4fd7-8030-7065044e798d</t>
+    <t>org.openqa.selenium.TimeoutException: Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.xpath: //android.widget.TextView[@resource-id='com.zopsmart.stg.scarlet:id/tv_page_name']' (tried for 20 second(s) with 500 milliseconds interval)</t>
   </si>
 </sst>
 </file>

</xml_diff>